<commit_message>
allow_registration (of students) disabled by default footer mailto link now includes subject with site name
</commit_message>
<xml_diff>
--- a/mod/z04_clipit_activity/vendors/templates/clipit_users.xlsx
+++ b/mod/z04_clipit_activity/vendors/templates/clipit_users.xlsx
@@ -152,16 +152,16 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -207,20 +207,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,164 +245,163 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="26" min="1" style="0" width="22.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="26" min="1" style="1" width="22.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="1" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>